<commit_message>
Updated change alm pw
</commit_message>
<xml_diff>
--- a/change alm pw/Default.xlsx
+++ b/change alm pw/Default.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="55">
   <si>
     <t>demo_val</t>
   </si>
@@ -90,6 +90,9 @@
   </si>
   <si>
     <t>mary_alm</t>
+  </si>
+  <si>
+    <t>admin</t>
   </si>
   <si>
     <t>demo_pl</t>
@@ -331,7 +334,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -342,9 +347,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -664,10 +667,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:B53"/>
+  <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:B53"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -677,325 +680,331 @@
     <col min="3" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1">
-      <c t="s">
+    <row r="1" customFormat="1">
+      <c r="A1" t="s">
+        <v>29</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B2" s="2"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B3" s="2"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B4" s="2"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="B5" s="2"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" s="2"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="B7" s="2"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="3" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="2"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="2"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B10" s="2"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="B11" s="2"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="B12" s="2"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B13" s="2"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B14" s="2"/>
+    </row>
+    <row r="15">
+      <c r="A15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B15" s="2"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="B16" s="2"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="B17" s="2"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" s="2"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="2"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="B20" s="2"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="2"/>
+    </row>
+    <row r="22">
+      <c r="A22" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="B22" s="2"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="B23" s="2"/>
+    </row>
+    <row r="24">
+      <c r="A24" s="3" t="s">
         <v>28</v>
       </c>
-      <c t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row>
-      <c s="2" t="s">
+      <c r="B24" s="2"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="B25" s="2"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26" s="2"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B27" s="2"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="3" t="s">
+        <v>53</v>
+      </c>
+      <c r="B28" s="2"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="B29" s="2"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="B30" s="2"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="B31" s="2"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="B32" s="2"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="B33" s="2"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B34" s="2"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B35" s="2"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B36" s="2"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B37" s="2"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="2"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="B39" s="2"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" s="2"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="B41" s="2"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="B42" s="2"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="B43" s="2"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B44" s="2"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B45" s="2"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B46" s="2"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B47" s="2"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B48" s="2"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B49" s="2"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="2"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="3" t="s">
         <v>35</v>
       </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>46</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>50</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>4</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>16</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>39</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>23</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>5</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>51</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>14</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>17</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>47</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>25</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>40</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>18</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>6</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>48</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>9</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>29</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>26</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>36</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>27</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>30</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>0</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>1</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>52</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>10</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>44</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>31</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>11</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>45</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>37</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>15</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>38</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>24</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>7</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>41</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>8</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>19</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>20</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>21</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>42</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>43</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>12</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>2</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>32</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>33</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>49</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>34</v>
-      </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
+      <c r="B51" s="2"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="3" t="s">
         <v>22</v>
       </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
+      <c r="B52" s="2"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="3" t="s">
         <v>13</v>
       </c>
-      <c s="3"/>
-    </row>
-    <row>
-      <c s="2" t="s">
-        <v>53</v>
-      </c>
-      <c s="3"/>
+      <c r="B53" s="2"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="B54" s="2"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1015,7 +1024,7 @@
     <col min="1" max="16384" width="9.078125" style="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row customFormat="1"/>
+    <row r="1" ht="14.95" customFormat="1"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Ron added loop to change alm pw test
</commit_message>
<xml_diff>
--- a/change alm pw/Default.xlsx
+++ b/change alm pw/Default.xlsx
@@ -92,16 +92,16 @@
     <t>mary_alm</t>
   </si>
   <si>
+    <t>demo_pl</t>
+  </si>
+  <si>
+    <t>demo_so</t>
+  </si>
+  <si>
+    <t>demo_tll</t>
+  </si>
+  <si>
     <t>admin</t>
-  </si>
-  <si>
-    <t>demo_pl</t>
-  </si>
-  <si>
-    <t>demo_so</t>
-  </si>
-  <si>
-    <t>demo_tll</t>
   </si>
   <si>
     <t>UserName</t>
@@ -334,9 +334,7 @@
     </border>
     <border>
       <left/>
-      <right style="thin">
-        <color rgb="FF000000"/>
-      </right>
+      <right/>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -347,7 +345,9 @@
     </border>
     <border>
       <left/>
-      <right/>
+      <right style="thin">
+        <color rgb="FF000000"/>
+      </right>
       <top style="thin">
         <color rgb="FF000000"/>
       </top>
@@ -670,7 +670,7 @@
   <dimension ref="A1:B54"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="A2" sqref="A2:XFD2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
@@ -689,322 +689,322 @@
       </c>
     </row>
     <row r="2">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="B2" s="3"/>
+    </row>
+    <row r="3">
+      <c r="A3" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="3"/>
+    </row>
+    <row r="4">
+      <c r="A4" s="2" t="s">
+        <v>51</v>
+      </c>
+      <c r="B4" s="3"/>
+    </row>
+    <row r="5">
+      <c r="A5" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" s="3"/>
+    </row>
+    <row r="6">
+      <c r="A6" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="3"/>
+    </row>
+    <row r="7">
+      <c r="A7" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="B7" s="3"/>
+    </row>
+    <row r="8">
+      <c r="A8" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B8" s="3"/>
+    </row>
+    <row r="9">
+      <c r="A9" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="3"/>
+    </row>
+    <row r="10">
+      <c r="A10" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="B10" s="3"/>
+    </row>
+    <row r="11">
+      <c r="A11" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B11" s="3"/>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B12" s="3"/>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="s">
+        <v>48</v>
+      </c>
+      <c r="B13" s="3"/>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="s">
         <v>25</v>
       </c>
-      <c r="B2" s="2"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="3" t="s">
-        <v>36</v>
-      </c>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4">
-      <c r="A4" s="3" t="s">
-        <v>47</v>
-      </c>
-      <c r="B4" s="2"/>
-    </row>
-    <row r="5">
-      <c r="A5" s="3" t="s">
-        <v>51</v>
-      </c>
-      <c r="B5" s="2"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="B6" s="2"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="B7" s="2"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="3" t="s">
-        <v>40</v>
-      </c>
-      <c r="B8" s="2"/>
-    </row>
-    <row r="9">
-      <c r="A9" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="B9" s="2"/>
-    </row>
-    <row r="10">
-      <c r="A10" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="B10" s="2"/>
-    </row>
-    <row r="11">
-      <c r="A11" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="B11" s="2"/>
-    </row>
-    <row r="12">
-      <c r="A12" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="B12" s="2"/>
-    </row>
-    <row r="13">
-      <c r="A13" s="3" t="s">
-        <v>17</v>
-      </c>
-      <c r="B13" s="2"/>
-    </row>
-    <row r="14">
-      <c r="A14" s="3" t="s">
-        <v>48</v>
-      </c>
-      <c r="B14" s="2"/>
+      <c r="B14" s="3"/>
     </row>
     <row r="15">
-      <c r="A15" s="3" t="s">
+      <c r="A15" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="3"/>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="B16" s="3"/>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" s="3"/>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="B18" s="3"/>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="B19" s="3"/>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3"/>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="s">
         <v>26</v>
       </c>
-      <c r="B15" s="2"/>
-    </row>
-    <row r="16">
-      <c r="A16" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="B16" s="2"/>
-    </row>
-    <row r="17">
-      <c r="A17" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="B17" s="2"/>
-    </row>
-    <row r="18">
-      <c r="A18" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" s="2"/>
-    </row>
-    <row r="19">
-      <c r="A19" s="3" t="s">
-        <v>49</v>
-      </c>
-      <c r="B19" s="2"/>
-    </row>
-    <row r="20">
-      <c r="A20" s="3" t="s">
-        <v>9</v>
-      </c>
-      <c r="B20" s="2"/>
-    </row>
-    <row r="21">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="2"/>
+      <c r="B21" s="3"/>
     </row>
     <row r="22">
-      <c r="A22" s="3" t="s">
+      <c r="A22" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="B22" s="3"/>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="s">
         <v>27</v>
       </c>
-      <c r="B22" s="2"/>
-    </row>
-    <row r="23">
-      <c r="A23" s="3" t="s">
-        <v>37</v>
-      </c>
-      <c r="B23" s="2"/>
+      <c r="B23" s="3"/>
     </row>
     <row r="24">
-      <c r="A24" s="3" t="s">
+      <c r="A24" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="B24" s="3"/>
+    </row>
+    <row r="25">
+      <c r="A25" s="2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25" s="3"/>
+    </row>
+    <row r="26">
+      <c r="A26" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="B26" s="3"/>
+    </row>
+    <row r="27">
+      <c r="A27" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="B27" s="3"/>
+    </row>
+    <row r="28">
+      <c r="A28" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="B28" s="3"/>
+    </row>
+    <row r="29">
+      <c r="A29" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="B29" s="3"/>
+    </row>
+    <row r="30">
+      <c r="A30" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="B30" s="3"/>
+    </row>
+    <row r="31">
+      <c r="A31" s="2" t="s">
+        <v>11</v>
+      </c>
+      <c r="B31" s="3"/>
+    </row>
+    <row r="32">
+      <c r="A32" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="B32" s="3"/>
+    </row>
+    <row r="33">
+      <c r="A33" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="B33" s="3"/>
+    </row>
+    <row r="34">
+      <c r="A34" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B34" s="3"/>
+    </row>
+    <row r="35">
+      <c r="A35" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="B35" s="3"/>
+    </row>
+    <row r="36">
+      <c r="A36" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="B36" s="3"/>
+    </row>
+    <row r="37">
+      <c r="A37" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="3"/>
+    </row>
+    <row r="38">
+      <c r="A38" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="B38" s="3"/>
+    </row>
+    <row r="39">
+      <c r="A39" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="B39" s="3"/>
+    </row>
+    <row r="40">
+      <c r="A40" s="2" t="s">
+        <v>19</v>
+      </c>
+      <c r="B40" s="3"/>
+    </row>
+    <row r="41">
+      <c r="A41" s="2" t="s">
+        <v>20</v>
+      </c>
+      <c r="B41" s="3"/>
+    </row>
+    <row r="42">
+      <c r="A42" s="2" t="s">
+        <v>21</v>
+      </c>
+      <c r="B42" s="3"/>
+    </row>
+    <row r="43">
+      <c r="A43" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="B43" s="3"/>
+    </row>
+    <row r="44">
+      <c r="A44" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="B44" s="3"/>
+    </row>
+    <row r="45">
+      <c r="A45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B45" s="3"/>
+    </row>
+    <row r="46">
+      <c r="A46" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B46" s="3"/>
+    </row>
+    <row r="47">
+      <c r="A47" s="2" t="s">
+        <v>33</v>
+      </c>
+      <c r="B47" s="3"/>
+    </row>
+    <row r="48">
+      <c r="A48" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="B48" s="3"/>
+    </row>
+    <row r="49">
+      <c r="A49" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="3"/>
+    </row>
+    <row r="50">
+      <c r="A50" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="B50" s="3"/>
+    </row>
+    <row r="51">
+      <c r="A51" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="B51" s="3"/>
+    </row>
+    <row r="52">
+      <c r="A52" s="2" t="s">
+        <v>13</v>
+      </c>
+      <c r="B52" s="3"/>
+    </row>
+    <row r="53">
+      <c r="A53" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="B53" s="3"/>
+    </row>
+    <row r="54">
+      <c r="A54" s="2" t="s">
         <v>28</v>
       </c>
-      <c r="B24" s="2"/>
-    </row>
-    <row r="25">
-      <c r="A25" s="3" t="s">
-        <v>31</v>
-      </c>
-      <c r="B25" s="2"/>
-    </row>
-    <row r="26">
-      <c r="A26" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26" s="2"/>
-    </row>
-    <row r="27">
-      <c r="A27" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="B27" s="2"/>
-    </row>
-    <row r="28">
-      <c r="A28" s="3" t="s">
-        <v>53</v>
-      </c>
-      <c r="B28" s="2"/>
-    </row>
-    <row r="29">
-      <c r="A29" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="B29" s="2"/>
-    </row>
-    <row r="30">
-      <c r="A30" s="3" t="s">
-        <v>45</v>
-      </c>
-      <c r="B30" s="2"/>
-    </row>
-    <row r="31">
-      <c r="A31" s="3" t="s">
-        <v>32</v>
-      </c>
-      <c r="B31" s="2"/>
-    </row>
-    <row r="32">
-      <c r="A32" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="B32" s="2"/>
-    </row>
-    <row r="33">
-      <c r="A33" s="3" t="s">
-        <v>46</v>
-      </c>
-      <c r="B33" s="2"/>
-    </row>
-    <row r="34">
-      <c r="A34" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B34" s="2"/>
-    </row>
-    <row r="35">
-      <c r="A35" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="B35" s="2"/>
-    </row>
-    <row r="36">
-      <c r="A36" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B36" s="2"/>
-    </row>
-    <row r="37">
-      <c r="A37" s="3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B37" s="2"/>
-    </row>
-    <row r="38">
-      <c r="A38" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="2"/>
-    </row>
-    <row r="39">
-      <c r="A39" s="3" t="s">
-        <v>42</v>
-      </c>
-      <c r="B39" s="2"/>
-    </row>
-    <row r="40">
-      <c r="A40" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B40" s="2"/>
-    </row>
-    <row r="41">
-      <c r="A41" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="B41" s="2"/>
-    </row>
-    <row r="42">
-      <c r="A42" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B42" s="2"/>
-    </row>
-    <row r="43">
-      <c r="A43" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="B43" s="2"/>
-    </row>
-    <row r="44">
-      <c r="A44" s="3" t="s">
-        <v>43</v>
-      </c>
-      <c r="B44" s="2"/>
-    </row>
-    <row r="45">
-      <c r="A45" s="3" t="s">
-        <v>44</v>
-      </c>
-      <c r="B45" s="2"/>
-    </row>
-    <row r="46">
-      <c r="A46" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B46" s="2"/>
-    </row>
-    <row r="47">
-      <c r="A47" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B47" s="2"/>
-    </row>
-    <row r="48">
-      <c r="A48" s="3" t="s">
-        <v>33</v>
-      </c>
-      <c r="B48" s="2"/>
-    </row>
-    <row r="49">
-      <c r="A49" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="B49" s="2"/>
-    </row>
-    <row r="50">
-      <c r="A50" s="3" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="2"/>
-    </row>
-    <row r="51">
-      <c r="A51" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="B51" s="2"/>
-    </row>
-    <row r="52">
-      <c r="A52" s="3" t="s">
-        <v>22</v>
-      </c>
-      <c r="B52" s="2"/>
-    </row>
-    <row r="53">
-      <c r="A53" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="B53" s="2"/>
-    </row>
-    <row r="54">
-      <c r="A54" s="3" t="s">
-        <v>54</v>
-      </c>
-      <c r="B54" s="2"/>
+      <c r="B54" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>